<commit_message>
Speed of Float Functions: update at time of post.
</commit_message>
<xml_diff>
--- a/2017-02-07 Faster Float Functions/2017-02 Speed of Float Functions.xlsx
+++ b/2017-02-07 Faster Float Functions/2017-02 Speed of Float Functions.xlsx
@@ -159,9 +159,9 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="168" formatCode="0.0\x"/>
+    <numFmt numFmtId="166" formatCode="0.0\x"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,8 +192,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,6 +236,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -256,7 +301,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -293,7 +338,7 @@
     <xf numFmtId="1" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -302,7 +347,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -314,6 +359,31 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,7 +507,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Pretty!$E$6:$E$10</c:f>
+              <c:f>Pretty!$F$6:$F$10</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="5"/>
@@ -469,11 +539,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="18071552"/>
-        <c:axId val="18073088"/>
+        <c:axId val="265825664"/>
+        <c:axId val="265835648"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="18071552"/>
+        <c:axId val="265825664"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -492,7 +562,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="18073088"/>
+        <c:crossAx val="265835648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -500,7 +570,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="18073088"/>
+        <c:axId val="265835648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5000"/>
@@ -531,7 +601,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="18071552"/>
+        <c:crossAx val="265825664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -612,7 +682,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Pretty!$E$6:$E$10</c:f>
+              <c:f>Pretty!$F$6:$F$10</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="5"/>
@@ -667,7 +737,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Pretty!$E$12:$E$16</c:f>
+              <c:f>Pretty!$F$12:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="5"/>
@@ -690,11 +760,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="138533888"/>
-        <c:axId val="138537216"/>
+        <c:axId val="265854976"/>
+        <c:axId val="265856512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="138533888"/>
+        <c:axId val="265854976"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -713,7 +783,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="138537216"/>
+        <c:crossAx val="265856512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -721,7 +791,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="138537216"/>
+        <c:axId val="265856512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -759,7 +829,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="138533888"/>
+        <c:crossAx val="265854976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -928,11 +998,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="256388096"/>
-        <c:axId val="256406272"/>
+        <c:axId val="265594368"/>
+        <c:axId val="265595904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="256388096"/>
+        <c:axId val="265594368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -941,7 +1011,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="256406272"/>
+        <c:crossAx val="265595904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -949,7 +1019,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="256406272"/>
+        <c:axId val="265595904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -960,7 +1030,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="256388096"/>
+        <c:crossAx val="265594368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1069,11 +1139,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="256430464"/>
-        <c:axId val="256432000"/>
+        <c:axId val="265632384"/>
+        <c:axId val="265634176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="256430464"/>
+        <c:axId val="265632384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1082,7 +1152,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="256432000"/>
+        <c:crossAx val="265634176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1090,7 +1160,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="256432000"/>
+        <c:axId val="265634176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1101,14 +1171,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="256430464"/>
+        <c:crossAx val="265632384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1329,11 +1398,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="267864320"/>
-        <c:axId val="267866112"/>
+        <c:axId val="265667712"/>
+        <c:axId val="265669248"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="267864320"/>
+        <c:axId val="265667712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1342,7 +1411,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="267866112"/>
+        <c:crossAx val="265669248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1350,7 +1419,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="267866112"/>
+        <c:axId val="265669248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1378,14 +1447,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="267864320"/>
+        <c:crossAx val="265667712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1621,11 +1689,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="260854528"/>
-        <c:axId val="260856064"/>
+        <c:axId val="266479872"/>
+        <c:axId val="266489856"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="260854528"/>
+        <c:axId val="266479872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1634,7 +1702,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="260856064"/>
+        <c:crossAx val="266489856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1642,7 +1710,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="260856064"/>
+        <c:axId val="266489856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1671,7 +1739,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="260854528"/>
+        <c:crossAx val="266479872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1703,13 +1771,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>157161</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>476249</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>90487</xdr:rowOff>
@@ -1733,13 +1801,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>442913</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
@@ -2218,24 +2286,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:K34"/>
+  <dimension ref="B3:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.125" customWidth="1"/>
-    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.875" customWidth="1"/>
-    <col min="6" max="6" width="1.25" customWidth="1"/>
-    <col min="8" max="8" width="2.25" customWidth="1"/>
-    <col min="9" max="9" width="17.625" customWidth="1"/>
-    <col min="10" max="11" width="10.25" customWidth="1"/>
+    <col min="2" max="3" width="11.625" customWidth="1"/>
+    <col min="4" max="4" width="0.75" customWidth="1"/>
+    <col min="5" max="6" width="11.625" customWidth="1"/>
+    <col min="7" max="7" width="0.75" customWidth="1"/>
+    <col min="8" max="8" width="9.5" customWidth="1"/>
+    <col min="9" max="9" width="2.25" customWidth="1"/>
+    <col min="10" max="10" width="17.625" customWidth="1"/>
+    <col min="11" max="12" width="10.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" s="29" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12" s="29" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="30" t="s">
         <v>44</v>
       </c>
@@ -2248,290 +2317,303 @@
       <c r="I3" s="30"/>
       <c r="J3" s="30"/>
       <c r="K3" s="30"/>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="18" t="s">
+      <c r="L3" s="30"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="40"/>
+      <c r="E5" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="F5" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="38"/>
+      <c r="H5" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="18" t="s">
+      <c r="J5" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="19" t="s">
+      <c r="K5" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="K5" s="19" t="s">
+      <c r="L5" s="19" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="15" t="str">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="31" t="str">
         <f>Raw!B57</f>
         <v>sqrt(x)</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="32">
         <f>AVERAGE(Raw!C40:D40)</f>
         <v>1348.5</v>
       </c>
-      <c r="D6" s="15" t="str">
+      <c r="D6" s="41"/>
+      <c r="E6" s="31" t="str">
         <f>Raw!B45</f>
         <v>sqrtf(x)</v>
       </c>
-      <c r="E6" s="17">
+      <c r="F6" s="32">
         <f>AVERAGE(Raw!C45:D45)</f>
         <v>43.2</v>
       </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="22">
-        <f>C6/E6</f>
+      <c r="G6" s="31"/>
+      <c r="H6" s="33">
+        <f>C6/F6</f>
         <v>31.215277777777775</v>
       </c>
-      <c r="I6" s="15" t="s">
+      <c r="J6" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="17">
+      <c r="K6" s="17">
         <f>AVERAGE(Raw!C48:D48)</f>
         <v>350.43</v>
       </c>
-      <c r="K6" s="16"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="15" t="str">
+      <c r="L6" s="16"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="31" t="str">
         <f>Raw!B58</f>
         <v>log(x)</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="32">
         <f>AVERAGE(Raw!C41:D41)</f>
         <v>3553</v>
       </c>
-      <c r="D7" s="15" t="str">
+      <c r="D7" s="41"/>
+      <c r="E7" s="31" t="str">
         <f>Raw!B46</f>
         <v>logf(x)</v>
       </c>
-      <c r="E7" s="17">
+      <c r="F7" s="32">
         <f>AVERAGE(Raw!C46:D46)</f>
         <v>288.625</v>
       </c>
-      <c r="F7" s="15"/>
-      <c r="G7" s="22">
-        <f t="shared" ref="G7:G16" si="0">C7/E7</f>
+      <c r="G7" s="31"/>
+      <c r="H7" s="33">
+        <f t="shared" ref="H7:H16" si="0">C7/F7</f>
         <v>12.310090948462538</v>
       </c>
-      <c r="I7" s="15" t="s">
+      <c r="J7" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="J7" s="17">
+      <c r="K7" s="17">
         <f>AVERAGE(Raw!C49:D49)</f>
         <v>124.48</v>
       </c>
-      <c r="K7" s="23">
-        <f>J6/J7</f>
+      <c r="L7" s="23">
+        <f>K6/K7</f>
         <v>2.8151510282776351</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="15" t="str">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="31" t="str">
         <f>Raw!B59</f>
         <v>exp(x)</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="32">
         <f>AVERAGE(Raw!C42:D42)</f>
         <v>2943</v>
       </c>
-      <c r="D8" s="15" t="str">
+      <c r="D8" s="41"/>
+      <c r="E8" s="31" t="str">
         <f>Raw!B47</f>
         <v>expf(x)</v>
       </c>
-      <c r="E8" s="17">
+      <c r="F8" s="32">
         <f>AVERAGE(Raw!C47:D47)</f>
         <v>270.92500000000001</v>
       </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="22">
+      <c r="G8" s="31"/>
+      <c r="H8" s="33">
         <f t="shared" si="0"/>
         <v>10.862784903571098</v>
       </c>
-      <c r="I8" s="18" t="s">
+      <c r="J8" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="J8" s="21" t="s">
+      <c r="K8" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="K8" s="19" t="s">
+      <c r="L8" s="19" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="15" t="str">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="31" t="str">
         <f>Raw!B60</f>
         <v>log10(x)</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="32">
         <f>AVERAGE(Raw!C43:D43)</f>
         <v>3452</v>
       </c>
-      <c r="D9" s="15" t="str">
+      <c r="D9" s="41"/>
+      <c r="E9" s="31" t="str">
         <f>Raw!B48</f>
         <v>log10f(x)</v>
       </c>
-      <c r="E9" s="17">
+      <c r="F9" s="32">
         <f>AVERAGE(Raw!C48:D48)</f>
         <v>350.43</v>
       </c>
-      <c r="F9" s="15"/>
-      <c r="G9" s="22">
+      <c r="G9" s="31"/>
+      <c r="H9" s="33">
         <f t="shared" si="0"/>
         <v>9.850754786976001</v>
       </c>
-      <c r="I9" s="15" t="s">
+      <c r="J9" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="17">
+      <c r="K9" s="17">
         <f>AVERAGE(Raw!C51:D51)</f>
         <v>859.7</v>
       </c>
-      <c r="K9" s="16"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="15" t="str">
+      <c r="L9" s="16"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="31" t="str">
         <f>Raw!B61</f>
         <v>pow(10.0,x)</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="32">
         <f>AVERAGE(Raw!C44:D44)</f>
         <v>9915.5</v>
       </c>
-      <c r="D10" s="15" t="str">
+      <c r="D10" s="41"/>
+      <c r="E10" s="31" t="str">
         <f>Raw!B51</f>
         <v>powf(10.0,x)</v>
       </c>
-      <c r="E10" s="17">
+      <c r="F10" s="32">
         <f>AVERAGE(Raw!C51:D51)</f>
         <v>859.7</v>
       </c>
-      <c r="F10" s="15"/>
-      <c r="G10" s="22">
+      <c r="G10" s="31"/>
+      <c r="H10" s="33">
         <f t="shared" si="0"/>
         <v>11.533674537629405</v>
       </c>
-      <c r="I10" s="15" t="s">
+      <c r="J10" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="J10" s="17">
+      <c r="K10" s="17">
         <f>AVERAGE(Raw!C52:D52)</f>
         <v>286.67500000000001</v>
       </c>
-      <c r="K10" s="23">
-        <f>J9/J10</f>
+      <c r="L10" s="23">
+        <f>K9/K10</f>
         <v>2.9988663120258132</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="8"/>
       <c r="C11" s="24"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="28"/>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D11" s="24"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="28"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="8"/>
       <c r="C12" s="24"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="28"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D12" s="24"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="28"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="8"/>
       <c r="C13" s="24"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="28"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="G14" s="26"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="28"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="H14" s="26"/>
       <c r="I14" s="26"/>
       <c r="J14" s="26"/>
       <c r="K14" s="26"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L14" s="26"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" t="str">
-        <f>D9</f>
+        <f>E9</f>
         <v>log10f(x)</v>
       </c>
       <c r="C15" s="14">
-        <f>E9</f>
+        <f>F9</f>
         <v>350.43</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="14"/>
+      <c r="E15" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="14">
+      <c r="F15" s="14">
         <f>AVERAGE(Raw!C49:D49)</f>
         <v>124.48</v>
       </c>
-      <c r="G15" s="22">
+      <c r="H15" s="22">
         <f t="shared" si="0"/>
         <v>2.8151510282776351</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" t="str">
-        <f>D10</f>
+        <f>E10</f>
         <v>powf(10.0,x)</v>
       </c>
       <c r="C16" s="14">
-        <f>E10</f>
+        <f>F10</f>
         <v>859.7</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="14"/>
+      <c r="E16" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="14">
+      <c r="F16" s="14">
         <f>AVERAGE(Raw!C52:D52)</f>
         <v>286.67500000000001</v>
       </c>
-      <c r="G16" s="22">
+      <c r="H16" s="22">
         <f t="shared" si="0"/>
         <v>2.9988663120258132</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="2">
         <v>180000000</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>5</v>
       </c>
@@ -2539,188 +2621,193 @@
         <v>44100</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" t="str">
-        <f>B5</f>
+        <f t="shared" ref="B21:B26" si="1">B5</f>
         <v>Function</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
       </c>
-      <c r="D21" t="str">
-        <f>D5</f>
+      <c r="E21" t="str">
+        <f t="shared" ref="E21:E26" si="2">E5</f>
         <v>Function</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>6</v>
       </c>
-      <c r="F21">
-        <f>F5</f>
+      <c r="G21">
+        <f>G5</f>
         <v>0</v>
       </c>
-      <c r="G21" s="13" t="str">
-        <f>G5</f>
+      <c r="H21" s="13" t="str">
+        <f>H5</f>
         <v>Speed Up</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" t="str">
-        <f>B6</f>
+        <f t="shared" si="1"/>
         <v>sqrt(x)</v>
       </c>
       <c r="C22" s="12">
         <f>$C$18/$C$19/C6</f>
         <v>3.0267947000824802</v>
       </c>
-      <c r="D22" t="str">
-        <f>D6</f>
+      <c r="D22" s="12"/>
+      <c r="E22" t="str">
+        <f t="shared" si="2"/>
         <v>sqrtf(x)</v>
       </c>
-      <c r="E22" s="12">
-        <f>$C$18/$C$19/E6</f>
+      <c r="F22" s="12">
+        <f>$C$18/$C$19/F6</f>
         <v>94.482237339380191</v>
       </c>
-      <c r="F22">
-        <f>F6</f>
+      <c r="G22">
+        <f>G6</f>
         <v>0</v>
       </c>
-      <c r="G22" s="20">
-        <f>E22/C22</f>
+      <c r="H22" s="20">
+        <f>F22/C22</f>
         <v>31.215277777777775</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" t="str">
-        <f>B7</f>
+        <f t="shared" si="1"/>
         <v>log(x)</v>
       </c>
       <c r="C23" s="12">
         <f>$C$18/$C$19/C7</f>
         <v>1.148784872800795</v>
       </c>
-      <c r="D23" t="str">
-        <f>D7</f>
+      <c r="D23" s="12"/>
+      <c r="E23" t="str">
+        <f t="shared" si="2"/>
         <v>logf(x)</v>
       </c>
-      <c r="E23" s="12">
-        <f>$C$18/$C$19/E7</f>
+      <c r="F23" s="12">
+        <f>$C$18/$C$19/F7</f>
         <v>14.141646264395755</v>
       </c>
-      <c r="F23">
-        <f>F7</f>
+      <c r="G23">
+        <f>G7</f>
         <v>0</v>
       </c>
-      <c r="G23" s="20">
-        <f t="shared" ref="G23:G26" si="1">E23/C23</f>
+      <c r="H23" s="20">
+        <f t="shared" ref="H23:H26" si="3">F23/C23</f>
         <v>12.310090948462538</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" t="str">
-        <f>B8</f>
+        <f t="shared" si="1"/>
         <v>exp(x)</v>
       </c>
       <c r="C24" s="12">
         <f>$C$18/$C$19/C8</f>
         <v>1.3868952270000763</v>
       </c>
-      <c r="D24" t="str">
-        <f>D8</f>
+      <c r="D24" s="12"/>
+      <c r="E24" t="str">
+        <f t="shared" si="2"/>
         <v>expf(x)</v>
       </c>
-      <c r="E24" s="12">
-        <f>$C$18/$C$19/E8</f>
+      <c r="F24" s="12">
+        <f>$C$18/$C$19/F8</f>
         <v>15.065544534691242</v>
       </c>
-      <c r="F24">
-        <f>F8</f>
+      <c r="G24">
+        <f>G8</f>
         <v>0</v>
       </c>
-      <c r="G24" s="20">
+      <c r="H24" s="20">
+        <f t="shared" si="3"/>
+        <v>10.8627849035711</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" t="str">
         <f t="shared" si="1"/>
-        <v>10.8627849035711</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" t="str">
-        <f>B9</f>
         <v>log10(x)</v>
       </c>
       <c r="C25" s="12">
         <f>$C$18/$C$19/C9</f>
         <v>1.1823964811880721</v>
       </c>
-      <c r="D25" t="str">
-        <f>D9</f>
+      <c r="D25" s="12"/>
+      <c r="E25" t="str">
+        <f t="shared" si="2"/>
         <v>log10f(x)</v>
       </c>
-      <c r="E25" s="12">
-        <f>$C$18/$C$19/E9</f>
+      <c r="F25" s="12">
+        <f>$C$18/$C$19/F9</f>
         <v>11.647497797166979</v>
       </c>
-      <c r="F25">
-        <f>F9</f>
+      <c r="G25">
+        <f>G9</f>
         <v>0</v>
       </c>
-      <c r="G25" s="20">
+      <c r="H25" s="20">
+        <f t="shared" si="3"/>
+        <v>9.850754786976001</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" t="str">
         <f t="shared" si="1"/>
-        <v>9.850754786976001</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" t="str">
-        <f>B10</f>
         <v>pow(10.0,x)</v>
       </c>
       <c r="C26" s="12">
         <f>$C$18/$C$19/C10</f>
         <v>0.41164163713995505</v>
       </c>
-      <c r="D26" t="str">
-        <f>D10</f>
+      <c r="D26" s="12"/>
+      <c r="E26" t="str">
+        <f t="shared" si="2"/>
         <v>powf(10.0,x)</v>
       </c>
-      <c r="E26" s="12">
-        <f>$C$18/$C$19/E10</f>
+      <c r="F26" s="12">
+        <f>$C$18/$C$19/F10</f>
         <v>4.7477406689091826</v>
       </c>
-      <c r="F26">
-        <f>F10</f>
+      <c r="G26">
+        <f>G10</f>
         <v>0</v>
       </c>
-      <c r="G26" s="20">
-        <f t="shared" si="1"/>
+      <c r="H26" s="20">
+        <f t="shared" si="3"/>
         <v>11.533674537629405</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G27" s="20"/>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H27" s="20"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" t="str">
         <f>B22</f>
         <v>sqrt(x)</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" t="str">
-        <f t="shared" ref="B31:B32" si="2">B23</f>
+        <f t="shared" ref="B31:B32" si="4">B23</f>
         <v>log(x)</v>
       </c>
-      <c r="E31">
+      <c r="F31">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>exp(x)</v>
       </c>
-      <c r="E32">
+      <c r="F32">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" t="str">
         <f>B15</f>
         <v>log10f(x)</v>
@@ -2729,24 +2816,25 @@
         <f>$C$18/$C$19/C15</f>
         <v>11.647497797166979</v>
       </c>
-      <c r="D33" t="str">
-        <f>D15</f>
+      <c r="D33" s="12"/>
+      <c r="E33" t="str">
+        <f>E15</f>
         <v>apprx_log10</v>
       </c>
-      <c r="E33" s="12">
-        <f>$C$18/$C$19/E15</f>
+      <c r="F33" s="12">
+        <f>$C$18/$C$19/F15</f>
         <v>32.789465400556111</v>
       </c>
-      <c r="F33">
-        <f>F15</f>
+      <c r="G33">
+        <f>G15</f>
         <v>0</v>
       </c>
-      <c r="G33" s="20">
-        <f>E33/C33</f>
+      <c r="H33" s="20">
+        <f>F33/C33</f>
         <v>2.8151510282776351</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" t="str">
         <f>B16</f>
         <v>powf(10.0,x)</v>
@@ -2755,20 +2843,21 @@
         <f>$C$18/$C$19/C16</f>
         <v>4.7477406689091826</v>
       </c>
-      <c r="D34" t="str">
-        <f>D16</f>
+      <c r="D34" s="12"/>
+      <c r="E34" t="str">
+        <f>E16</f>
         <v>exp(log(10*x)</v>
       </c>
-      <c r="E34" s="12">
-        <f>$C$18/$C$19/E16</f>
+      <c r="F34" s="12">
+        <f>$C$18/$C$19/F16</f>
         <v>14.237839550226647</v>
       </c>
-      <c r="F34">
-        <f>F16</f>
+      <c r="G34">
+        <f>G16</f>
         <v>0</v>
       </c>
-      <c r="G34" s="20">
-        <f>E34/C34</f>
+      <c r="H34" s="20">
+        <f>F34/C34</f>
         <v>2.9988663120258132</v>
       </c>
     </row>

</xml_diff>